<commit_message>
yb changed E/F locus to L/M in .xlsx sheet to match text
</commit_message>
<xml_diff>
--- a/writeup_and_notes/TransmissionRules.xlsx
+++ b/writeup_and_notes/TransmissionRules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" firstSheet="3" activeTab="5"/>
@@ -137,33 +137,6 @@
     <t>(d1/2)</t>
   </si>
   <si>
-    <t>AAEE</t>
-  </si>
-  <si>
-    <t>ABEE</t>
-  </si>
-  <si>
-    <t>BBEE</t>
-  </si>
-  <si>
-    <t>AAEF</t>
-  </si>
-  <si>
-    <t>ABEF</t>
-  </si>
-  <si>
-    <t>BBEF</t>
-  </si>
-  <si>
-    <t>AAFF</t>
-  </si>
-  <si>
-    <t>ABFF</t>
-  </si>
-  <si>
-    <t>BBFF</t>
-  </si>
-  <si>
     <t>((1-d0)/4+(1-d1)/4)</t>
   </si>
   <si>
@@ -214,6 +187,33 @@
   <si>
     <t>Kids(mat first for bookkeeping)</t>
   </si>
+  <si>
+    <t>AALL</t>
+  </si>
+  <si>
+    <t>ABLL</t>
+  </si>
+  <si>
+    <t>BBLL</t>
+  </si>
+  <si>
+    <t>AALM</t>
+  </si>
+  <si>
+    <t>ABLM</t>
+  </si>
+  <si>
+    <t>BBLM</t>
+  </si>
+  <si>
+    <t>AAMM</t>
+  </si>
+  <si>
+    <t>ABMM</t>
+  </si>
+  <si>
+    <t>BBMM</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +228,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1091,13 +1090,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
@@ -1109,17 +1101,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="480">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1940,45 +1939,45 @@
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="70"/>
+    <col min="3" max="3" width="10.83203125" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="A1" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
-      <c r="A2" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="83" t="s">
+      <c r="A2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="72">
         <v>1</v>
       </c>
       <c r="D3" s="23">
@@ -1989,13 +1988,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -2006,13 +2005,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="74" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2023,64 +2022,64 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="76" t="s">
-        <v>52</v>
+      <c r="C6" s="73" t="s">
+        <v>43</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>54</v>
+      <c r="C7" s="73" t="s">
+        <v>45</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="72" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="23" t="s">
@@ -2091,13 +2090,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="67" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -2108,13 +2107,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="26" t="s">
@@ -2152,45 +2151,45 @@
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="70"/>
+    <col min="3" max="3" width="10.83203125" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="A1" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
-      <c r="A2" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="83" t="s">
+      <c r="A2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="72">
         <v>1</v>
       </c>
       <c r="D3" s="23">
@@ -2201,13 +2200,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -2218,13 +2217,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="74" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2235,13 +2234,13 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -2252,47 +2251,47 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>54</v>
+      <c r="C7" s="73" t="s">
+        <v>45</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="72" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="23" t="s">
@@ -2303,13 +2302,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="67" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -2320,13 +2319,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="26" t="s">
@@ -2364,45 +2363,45 @@
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="70"/>
+    <col min="3" max="3" width="10.83203125" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
+      <c r="A1" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
-      <c r="A2" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="83" t="s">
+      <c r="A2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="75">
+      <c r="C3" s="72">
         <v>1</v>
       </c>
       <c r="D3" s="23">
@@ -2413,13 +2412,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="67" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -2430,13 +2429,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="74" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2447,13 +2446,13 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="73" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -2464,47 +2463,47 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>59</v>
+      <c r="C7" s="73" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="72" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="23" t="s">
@@ -2515,13 +2514,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="67" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -2532,13 +2531,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="6" customFormat="1" ht="16" thickBot="1">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="77" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="26" t="s">
@@ -2590,21 +2589,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="A1" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
     </row>
     <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" t="s">
@@ -3929,21 +3928,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
+      <c r="A1" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
     </row>
     <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" t="s">
@@ -5261,10 +5260,10 @@
   <dimension ref="A1:K175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5283,21 +5282,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1">
-      <c r="A1" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68" t="s">
+      <c r="A1" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="16" thickBot="1">
       <c r="A2" s="44" t="s">
@@ -5306,40 +5305,40 @@
       <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="87" t="s">
-        <v>37</v>
+      <c r="C2" s="81" t="s">
+        <v>54</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A3" s="34" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>8</v>
@@ -5371,10 +5370,10 @@
     </row>
     <row r="4" spans="1:11" s="39" customFormat="1">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C4" s="55" t="s">
         <v>6</v>
@@ -5406,10 +5405,10 @@
     </row>
     <row r="5" spans="1:11" s="39" customFormat="1">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C5" s="55" t="s">
         <v>7</v>
@@ -5441,10 +5440,10 @@
     </row>
     <row r="6" spans="1:11" s="39" customFormat="1">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>6</v>
@@ -5476,10 +5475,10 @@
     </row>
     <row r="7" spans="1:11" s="39" customFormat="1">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C7" s="55" t="s">
         <v>18</v>
@@ -5511,10 +5510,10 @@
     </row>
     <row r="8" spans="1:11" s="39" customFormat="1">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>7</v>
@@ -5546,10 +5545,10 @@
     </row>
     <row r="9" spans="1:11" s="39" customFormat="1">
       <c r="A9" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>7</v>
@@ -5581,10 +5580,10 @@
     </row>
     <row r="10" spans="1:11" s="39" customFormat="1">
       <c r="A10" s="17" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C10" s="55" t="s">
         <v>7</v>
@@ -5616,10 +5615,10 @@
     </row>
     <row r="11" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A11" s="33" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>7</v>
@@ -5651,10 +5650,10 @@
     </row>
     <row r="12" spans="1:11" ht="16" thickTop="1">
       <c r="A12" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>9</v>
@@ -5686,10 +5685,10 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C13" s="55" t="s">
         <v>11</v>
@@ -5721,10 +5720,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C14" s="55">
         <v>0</v>
@@ -5756,10 +5755,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C15" s="55" t="s">
         <v>11</v>
@@ -5791,10 +5790,10 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C16" s="55" t="s">
         <v>24</v>
@@ -5826,10 +5825,10 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C17" s="55" t="s">
         <v>7</v>
@@ -5861,10 +5860,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C18" s="55" t="s">
         <v>7</v>
@@ -5896,10 +5895,10 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="17" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C19" s="55" t="s">
         <v>7</v>
@@ -5931,10 +5930,10 @@
     </row>
     <row r="20" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A20" s="33" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C20" s="57" t="s">
         <v>7</v>
@@ -5966,10 +5965,10 @@
     </row>
     <row r="21" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A21" s="34" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C21" s="55" t="s">
         <v>7</v>
@@ -6001,10 +6000,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C22" s="55" t="s">
         <v>7</v>
@@ -6036,10 +6035,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>7</v>
@@ -6071,10 +6070,10 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>7</v>
@@ -6106,10 +6105,10 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B25" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C25" s="55" t="s">
         <v>7</v>
@@ -6141,10 +6140,10 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C26" s="55" t="s">
         <v>7</v>
@@ -6176,10 +6175,10 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>7</v>
@@ -6211,10 +6210,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C28" s="55" t="s">
         <v>7</v>
@@ -6246,10 +6245,10 @@
     </row>
     <row r="29" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A29" s="33" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C29" s="57" t="s">
         <v>7</v>
@@ -6281,10 +6280,10 @@
     </row>
     <row r="30" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A30" s="34" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C30" s="51" t="s">
         <v>6</v>
@@ -6316,10 +6315,10 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C31" s="55" t="s">
         <v>18</v>
@@ -6351,10 +6350,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C32" s="55" t="s">
         <v>7</v>
@@ -6386,10 +6385,10 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C33" s="55" t="s">
         <v>18</v>
@@ -6421,10 +6420,10 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B34" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C34" s="55" t="s">
         <v>29</v>
@@ -6456,10 +6455,10 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B35" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C35" s="55" t="s">
         <v>7</v>
@@ -6491,10 +6490,10 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B36" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C36" s="55" t="s">
         <v>7</v>
@@ -6526,10 +6525,10 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="17" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B37" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C37" s="55" t="s">
         <v>7</v>
@@ -6561,10 +6560,10 @@
     </row>
     <row r="38" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A38" s="33" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B38" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C38" s="57" t="s">
         <v>7</v>
@@ -6596,10 +6595,10 @@
     </row>
     <row r="39" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A39" s="34" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>11</v>
@@ -6631,10 +6630,10 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C40" s="55" t="s">
         <v>24</v>
@@ -6666,10 +6665,10 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B41" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C41" s="55" t="s">
         <v>7</v>
@@ -6701,10 +6700,10 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B42" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C42" s="55" t="s">
         <v>24</v>
@@ -6716,10 +6715,10 @@
         <v>7</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>7</v>
@@ -6736,10 +6735,10 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B43" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C43" s="55" t="s">
         <v>32</v>
@@ -6751,13 +6750,13 @@
         <v>33</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I43" s="60" t="s">
         <v>34</v>
@@ -6771,10 +6770,10 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B44" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C44" s="55" t="s">
         <v>7</v>
@@ -6789,10 +6788,10 @@
         <v>7</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I44" s="60" t="s">
         <v>7</v>
@@ -6806,10 +6805,10 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B45" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C45" s="55" t="s">
         <v>7</v>
@@ -6841,10 +6840,10 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="17" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B46" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C46" s="55" t="s">
         <v>7</v>
@@ -6876,10 +6875,10 @@
     </row>
     <row r="47" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A47" s="33" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C47" s="57" t="s">
         <v>7</v>
@@ -6911,10 +6910,10 @@
     </row>
     <row r="48" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A48" s="34" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>7</v>
@@ -6946,10 +6945,10 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B49" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C49" s="55" t="s">
         <v>7</v>
@@ -6981,10 +6980,10 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B50" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C50" s="55" t="s">
         <v>7</v>
@@ -7016,10 +7015,10 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B51" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C51" s="55" t="s">
         <v>7</v>
@@ -7051,10 +7050,10 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B52" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C52" s="55" t="s">
         <v>7</v>
@@ -7086,10 +7085,10 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B53" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C53" s="55" t="s">
         <v>7</v>
@@ -7121,10 +7120,10 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B54" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C54" s="55" t="s">
         <v>7</v>
@@ -7156,10 +7155,10 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="17" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B55" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C55" s="55" t="s">
         <v>7</v>
@@ -7191,10 +7190,10 @@
     </row>
     <row r="56" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A56" s="33" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B56" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C56" s="57" t="s">
         <v>7</v>
@@ -7226,10 +7225,10 @@
     </row>
     <row r="57" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A57" s="34" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C57" s="51">
         <v>0</v>
@@ -7261,10 +7260,10 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B58" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C58" s="55">
         <v>0</v>
@@ -7296,10 +7295,10 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B59" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C59" s="55">
         <v>0</v>
@@ -7331,10 +7330,10 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B60" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C60" s="55">
         <v>0</v>
@@ -7366,10 +7365,10 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B61" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C61" s="55">
         <v>0</v>
@@ -7401,10 +7400,10 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B62" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C62" s="55">
         <v>0</v>
@@ -7436,10 +7435,10 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B63" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C63" s="55">
         <v>0</v>
@@ -7471,10 +7470,10 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="17" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B64" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C64" s="55">
         <v>0</v>
@@ -7506,10 +7505,10 @@
     </row>
     <row r="65" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A65" s="33" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B65" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C65" s="57">
         <v>0</v>
@@ -7541,10 +7540,10 @@
     </row>
     <row r="66" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A66" s="34" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C66" s="51">
         <v>0</v>
@@ -7576,10 +7575,10 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B67" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C67" s="55">
         <v>0</v>
@@ -7611,10 +7610,10 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B68" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C68" s="55">
         <v>0</v>
@@ -7646,10 +7645,10 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B69" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C69" s="55">
         <v>0</v>
@@ -7681,10 +7680,10 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B70" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C70" s="55">
         <v>0</v>
@@ -7716,10 +7715,10 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C71" s="55">
         <v>0</v>
@@ -7751,10 +7750,10 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B72" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C72" s="55">
         <v>0</v>
@@ -7786,10 +7785,10 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="17" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B73" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C73" s="55">
         <v>0</v>
@@ -7821,10 +7820,10 @@
     </row>
     <row r="74" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A74" s="33" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B74" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C74" s="57">
         <v>0</v>
@@ -7851,15 +7850,15 @@
         <v>15</v>
       </c>
       <c r="K74" s="59" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="35" customFormat="1" ht="16" thickTop="1">
       <c r="A75" s="34" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C75" s="51">
         <v>0</v>
@@ -7891,10 +7890,10 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B76" s="54" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C76" s="55">
         <v>0</v>
@@ -7926,10 +7925,10 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B77" s="54" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C77" s="55">
         <v>0</v>
@@ -7961,10 +7960,10 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B78" s="54" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C78" s="55">
         <v>0</v>
@@ -7996,10 +7995,10 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B79" s="54" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C79" s="55">
         <v>0</v>
@@ -8031,10 +8030,10 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B80" s="54" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C80" s="55">
         <v>0</v>
@@ -8066,10 +8065,10 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B81" s="54" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C81" s="55">
         <v>0</v>
@@ -8101,10 +8100,10 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B82" s="54" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C82" s="55">
         <v>0</v>
@@ -8136,10 +8135,10 @@
     </row>
     <row r="83" spans="1:11" s="43" customFormat="1" ht="16" thickBot="1">
       <c r="A83" s="33" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B83" s="56" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C83" s="57">
         <v>0</v>

</xml_diff>

<commit_message>
working on trnasmission rules for unlinked female drive model
</commit_message>
<xml_diff>
--- a/writeup_and_notes/TransmissionRules.xlsx
+++ b/writeup_and_notes/TransmissionRules.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="40800" yWindow="1120" windowWidth="52360" windowHeight="16420" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model 1. Traditional driver" sheetId="7" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Model 4. Two-locus, coupling" sheetId="1" r:id="rId4"/>
     <sheet name="Model 5. Two-locus, repulsion" sheetId="3" r:id="rId5"/>
     <sheet name="Model 6. Two-locus, unlinked" sheetId="5" r:id="rId6"/>
+    <sheet name="Model 7. Two-locus unlinked fem" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="63">
   <si>
     <t>MOM</t>
   </si>
@@ -540,7 +541,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="480">
+  <cellStyleXfs count="482">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1020,6 +1021,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="88">
@@ -1120,7 +1123,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="480">
+  <cellStyles count="482">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1415,6 +1418,7 @@
     <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1600,6 +1604,7 @@
     <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5259,11 +5264,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A1:K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9287,4 +9292,2916 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" thickBot="1">
+      <c r="A2" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" thickTop="1">
+      <c r="A3" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" thickBot="1">
+      <c r="A11" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickTop="1">
+      <c r="A12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+      <c r="G12" s="17">
+        <v>0</v>
+      </c>
+      <c r="H12" s="31">
+        <v>0</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0</v>
+      </c>
+      <c r="K12" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="32">
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+      <c r="H13" s="31">
+        <v>0</v>
+      </c>
+      <c r="I13" s="60">
+        <v>0</v>
+      </c>
+      <c r="J13" s="60">
+        <v>0</v>
+      </c>
+      <c r="K13" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="55">
+        <v>0</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="32">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="31">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="31">
+        <v>0</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" thickBot="1">
+      <c r="A20" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" thickTop="1">
+      <c r="A21" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="34">
+        <v>1</v>
+      </c>
+      <c r="E21" s="34">
+        <v>0</v>
+      </c>
+      <c r="F21" s="32">
+        <v>0</v>
+      </c>
+      <c r="G21" s="34">
+        <v>0</v>
+      </c>
+      <c r="H21" s="53">
+        <v>0</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>0</v>
+      </c>
+      <c r="K21" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="32">
+        <v>0</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="60">
+        <v>0</v>
+      </c>
+      <c r="J22" s="60">
+        <v>0</v>
+      </c>
+      <c r="K22" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K23" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+      <c r="J24" s="17">
+        <v>0</v>
+      </c>
+      <c r="K24" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="32">
+        <v>0</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="32">
+        <v>0</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="32">
+        <v>0</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="32">
+        <v>0</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" thickBot="1">
+      <c r="A29" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="58">
+        <v>0</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" thickTop="1">
+      <c r="A30" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" thickBot="1">
+      <c r="A38" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="K38" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" thickTop="1">
+      <c r="A39" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="34">
+        <v>0</v>
+      </c>
+      <c r="F39" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="53">
+        <v>0</v>
+      </c>
+      <c r="I39" s="34">
+        <v>0</v>
+      </c>
+      <c r="J39" s="34">
+        <v>0</v>
+      </c>
+      <c r="K39" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="K42" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="J43" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="K43" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="K45" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="J46" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="16" thickBot="1">
+      <c r="A47" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="I47" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="K47" s="59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="16" thickTop="1">
+      <c r="A48" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="K52" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K55" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="16" thickBot="1">
+      <c r="A56" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K56" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="16" thickTop="1">
+      <c r="A57" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="51">
+        <v>0</v>
+      </c>
+      <c r="D57" s="34">
+        <v>0</v>
+      </c>
+      <c r="E57" s="34">
+        <v>0</v>
+      </c>
+      <c r="F57" s="52">
+        <v>1</v>
+      </c>
+      <c r="G57" s="34">
+        <v>0</v>
+      </c>
+      <c r="H57" s="53">
+        <v>0</v>
+      </c>
+      <c r="I57" s="34">
+        <v>0</v>
+      </c>
+      <c r="J57" s="34">
+        <v>0</v>
+      </c>
+      <c r="K57" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="55">
+        <v>0</v>
+      </c>
+      <c r="D58" s="17">
+        <v>0</v>
+      </c>
+      <c r="E58" s="17">
+        <v>0</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="60">
+        <v>0</v>
+      </c>
+      <c r="J58" s="60">
+        <v>0</v>
+      </c>
+      <c r="K58" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="55">
+        <v>0</v>
+      </c>
+      <c r="D59" s="17">
+        <v>0</v>
+      </c>
+      <c r="E59" s="17">
+        <v>0</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" s="60">
+        <v>0</v>
+      </c>
+      <c r="J59" s="60">
+        <v>0</v>
+      </c>
+      <c r="K59" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="55">
+        <v>0</v>
+      </c>
+      <c r="D60" s="17">
+        <v>0</v>
+      </c>
+      <c r="E60" s="17">
+        <v>0</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="55">
+        <v>0</v>
+      </c>
+      <c r="D61" s="17">
+        <v>0</v>
+      </c>
+      <c r="E61" s="17">
+        <v>0</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="55">
+        <v>0</v>
+      </c>
+      <c r="D62" s="17">
+        <v>0</v>
+      </c>
+      <c r="E62" s="17">
+        <v>0</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H62" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="55">
+        <v>0</v>
+      </c>
+      <c r="D63" s="17">
+        <v>0</v>
+      </c>
+      <c r="E63" s="17">
+        <v>0</v>
+      </c>
+      <c r="F63" s="32">
+        <v>0</v>
+      </c>
+      <c r="G63" s="17">
+        <v>0</v>
+      </c>
+      <c r="H63" s="31">
+        <v>0</v>
+      </c>
+      <c r="I63" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="J63" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="55">
+        <v>0</v>
+      </c>
+      <c r="D64" s="17">
+        <v>0</v>
+      </c>
+      <c r="E64" s="17">
+        <v>0</v>
+      </c>
+      <c r="F64" s="32">
+        <v>0</v>
+      </c>
+      <c r="G64" s="17">
+        <v>0</v>
+      </c>
+      <c r="H64" s="31">
+        <v>0</v>
+      </c>
+      <c r="I64" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J64" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K64" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="16" thickBot="1">
+      <c r="A65" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="57">
+        <v>0</v>
+      </c>
+      <c r="D65" s="33">
+        <v>0</v>
+      </c>
+      <c r="E65" s="33">
+        <v>0</v>
+      </c>
+      <c r="F65" s="58">
+        <v>0</v>
+      </c>
+      <c r="G65" s="33">
+        <v>0</v>
+      </c>
+      <c r="H65" s="59">
+        <v>0</v>
+      </c>
+      <c r="I65" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K65" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="16" thickTop="1">
+      <c r="A66" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="51">
+        <v>0</v>
+      </c>
+      <c r="D66" s="34">
+        <v>0</v>
+      </c>
+      <c r="E66" s="53">
+        <v>0</v>
+      </c>
+      <c r="F66" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I66" s="34">
+        <v>0</v>
+      </c>
+      <c r="J66" s="34">
+        <v>0</v>
+      </c>
+      <c r="K66" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" s="55">
+        <v>0</v>
+      </c>
+      <c r="D67" s="17">
+        <v>0</v>
+      </c>
+      <c r="E67" s="31">
+        <v>0</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I67" s="60">
+        <v>0</v>
+      </c>
+      <c r="J67" s="60">
+        <v>0</v>
+      </c>
+      <c r="K67" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="55">
+        <v>0</v>
+      </c>
+      <c r="D68" s="17">
+        <v>0</v>
+      </c>
+      <c r="E68" s="31">
+        <v>0</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I68" s="60">
+        <v>0</v>
+      </c>
+      <c r="J68" s="60">
+        <v>0</v>
+      </c>
+      <c r="K68" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" s="55">
+        <v>0</v>
+      </c>
+      <c r="D69" s="17">
+        <v>0</v>
+      </c>
+      <c r="E69" s="31">
+        <v>0</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I69" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="55">
+        <v>0</v>
+      </c>
+      <c r="D70" s="17">
+        <v>0</v>
+      </c>
+      <c r="E70" s="31">
+        <v>0</v>
+      </c>
+      <c r="F70" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="G70" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K70" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" s="55">
+        <v>0</v>
+      </c>
+      <c r="D71" s="17">
+        <v>0</v>
+      </c>
+      <c r="E71" s="31">
+        <v>0</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J71" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K71" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="55">
+        <v>0</v>
+      </c>
+      <c r="D72" s="17">
+        <v>0</v>
+      </c>
+      <c r="E72" s="31">
+        <v>0</v>
+      </c>
+      <c r="F72" s="17">
+        <v>0</v>
+      </c>
+      <c r="G72" s="17">
+        <v>0</v>
+      </c>
+      <c r="H72" s="31">
+        <v>0</v>
+      </c>
+      <c r="I72" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="55">
+        <v>0</v>
+      </c>
+      <c r="D73" s="17">
+        <v>0</v>
+      </c>
+      <c r="E73" s="31">
+        <v>0</v>
+      </c>
+      <c r="F73" s="17">
+        <v>0</v>
+      </c>
+      <c r="G73" s="17">
+        <v>0</v>
+      </c>
+      <c r="H73" s="31">
+        <v>0</v>
+      </c>
+      <c r="I73" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K73" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="16" thickBot="1">
+      <c r="A74" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="57">
+        <v>0</v>
+      </c>
+      <c r="D74" s="33">
+        <v>0</v>
+      </c>
+      <c r="E74" s="59">
+        <v>0</v>
+      </c>
+      <c r="F74" s="33">
+        <v>0</v>
+      </c>
+      <c r="G74" s="33">
+        <v>0</v>
+      </c>
+      <c r="H74" s="59">
+        <v>0</v>
+      </c>
+      <c r="I74" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J74" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="K74" s="59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="16" thickTop="1">
+      <c r="A75" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="51">
+        <v>0</v>
+      </c>
+      <c r="D75" s="34">
+        <v>0</v>
+      </c>
+      <c r="E75" s="53">
+        <v>0</v>
+      </c>
+      <c r="F75" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I75" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J75" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K75" s="53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="55">
+        <v>0</v>
+      </c>
+      <c r="D76" s="17">
+        <v>0</v>
+      </c>
+      <c r="E76" s="31">
+        <v>0</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I76" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J76" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K76" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="55">
+        <v>0</v>
+      </c>
+      <c r="D77" s="17">
+        <v>0</v>
+      </c>
+      <c r="E77" s="31">
+        <v>0</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J77" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K77" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" s="55">
+        <v>0</v>
+      </c>
+      <c r="D78" s="17">
+        <v>0</v>
+      </c>
+      <c r="E78" s="31">
+        <v>0</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J78" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K78" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="55">
+        <v>0</v>
+      </c>
+      <c r="D79" s="17">
+        <v>0</v>
+      </c>
+      <c r="E79" s="31">
+        <v>0</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I79" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J79" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K79" s="31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="55">
+        <v>0</v>
+      </c>
+      <c r="D80" s="17">
+        <v>0</v>
+      </c>
+      <c r="E80" s="31">
+        <v>0</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I80" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J80" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C81" s="55">
+        <v>0</v>
+      </c>
+      <c r="D81" s="17">
+        <v>0</v>
+      </c>
+      <c r="E81" s="31">
+        <v>0</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I81" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="K81" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="55">
+        <v>0</v>
+      </c>
+      <c r="D82" s="17">
+        <v>0</v>
+      </c>
+      <c r="E82" s="31">
+        <v>0</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H82" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I82" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J82" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="K82" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="16" thickBot="1">
+      <c r="A83" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B83" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" s="57">
+        <v>0</v>
+      </c>
+      <c r="D83" s="33">
+        <v>0</v>
+      </c>
+      <c r="E83" s="59">
+        <v>0</v>
+      </c>
+      <c r="F83" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G83" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="I83" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J83" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K83" s="59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="16" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
yb Added model 7 [female drive suppression] to TransmissionRules.xls
</commit_message>
<xml_diff>
--- a/writeup_and_notes/TransmissionRules.xlsx
+++ b/writeup_and_notes/TransmissionRules.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40800" yWindow="1120" windowWidth="52360" windowHeight="16420" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="729" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model 1. Traditional driver" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="87">
   <si>
     <t>MOM</t>
   </si>
@@ -215,6 +215,78 @@
   <si>
     <t>BBMM</t>
   </si>
+  <si>
+    <t>(d0)</t>
+  </si>
+  <si>
+    <t>(1/2)</t>
+  </si>
+  <si>
+    <t>((1-d0)/2)</t>
+  </si>
+  <si>
+    <t>((1-d0)/4)</t>
+  </si>
+  <si>
+    <t>(1/4)</t>
+  </si>
+  <si>
+    <t>((1-dh)/2)</t>
+  </si>
+  <si>
+    <t>((1-dh)/4)</t>
+  </si>
+  <si>
+    <t>(dh/2)</t>
+  </si>
+  <si>
+    <t>(dh/4)</t>
+  </si>
+  <si>
+    <t>(1/8)</t>
+  </si>
+  <si>
+    <t>((1-dh)/8)</t>
+  </si>
+  <si>
+    <t>(dh/8)</t>
+  </si>
+  <si>
+    <t>((1-d1)/2)</t>
+  </si>
+  <si>
+    <t>((1-d1)/4)</t>
+  </si>
+  <si>
+    <t>(d1/4)</t>
+  </si>
+  <si>
+    <t>AAEE</t>
+  </si>
+  <si>
+    <t>ABEE</t>
+  </si>
+  <si>
+    <t>BBEE</t>
+  </si>
+  <si>
+    <t>AAEF</t>
+  </si>
+  <si>
+    <t>ABEF</t>
+  </si>
+  <si>
+    <t>BBEF</t>
+  </si>
+  <si>
+    <t>AAFF</t>
+  </si>
+  <si>
+    <t>ABFF</t>
+  </si>
+  <si>
+    <t>BBFF</t>
+  </si>
 </sst>
 </file>
 
@@ -223,12 +295,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,6 +341,13 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="3">
@@ -541,7 +621,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="482">
+  <cellStyleXfs count="1116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1024,8 +1104,642 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1108,6 +1822,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1123,7 +1843,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="482">
+  <cellStyles count="1116">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1419,6 +2139,323 @@
     <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="493" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="495" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="497" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="499" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="805" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="807" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="809" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="811" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="813" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="815" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="817" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="819" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="821" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="823" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="825" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="837" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="839" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="841" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="843" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="845" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="847" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="849" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="851" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="853" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="855" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="857" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="859" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="861" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="863" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="865" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="867" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="887" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="889" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="891" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="893" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="895" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="897" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="899" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="901" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="903" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="905" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="907" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="909" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="911" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="913" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="915" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="917" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="919" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="921" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="923" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="925" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="927" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="929" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="931" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="933" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="935" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="937" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="939" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="941" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="943" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="945" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="947" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="949" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="951" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="953" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="955" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="957" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="959" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="961" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="963" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="965" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="967" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="969" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="971" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="973" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="975" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="977" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="979" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="981" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="983" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="985" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="987" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="989" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="991" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="993" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="995" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="997" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="999" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1001" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1003" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1005" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1007" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1009" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1011" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1013" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1015" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1017" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1019" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1021" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1023" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1025" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1027" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1029" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1031" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1033" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1035" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1037" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1039" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1041" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1043" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1045" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1047" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1049" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1051" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1053" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1055" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1057" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1059" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1061" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1063" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1065" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1067" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1069" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1071" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1073" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1075" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1077" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1079" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1081" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1083" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1085" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1087" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1089" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1091" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1093" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1095" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1097" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1099" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1115" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1605,6 +2642,323 @@
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="492" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="494" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="496" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="498" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="804" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="806" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="808" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="810" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="812" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="814" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="816" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="818" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="820" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="822" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="824" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="836" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="838" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="840" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="842" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="844" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="846" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="848" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="850" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="852" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="854" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="856" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="858" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="860" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="862" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="864" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="866" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="886" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="888" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="890" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="892" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="894" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="896" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="898" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="900" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="902" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="904" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="906" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="908" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="910" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="912" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="914" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="916" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="918" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="920" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="922" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="924" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="926" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="928" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="930" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="932" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="934" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="936" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="938" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="940" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="942" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="944" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="946" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="948" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="950" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="952" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="954" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="956" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="958" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="960" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="962" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="964" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="966" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="968" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="970" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="972" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="974" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="976" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="978" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="980" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="982" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="984" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="986" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="988" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="990" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="992" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="994" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="996" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="998" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1000" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1002" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1004" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1006" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1008" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1010" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1012" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1014" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1016" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1018" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1020" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1022" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1024" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1026" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1028" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1030" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1032" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1034" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1036" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1038" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1040" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1042" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1044" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1046" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1048" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1050" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1052" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1054" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1056" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1058" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1060" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1062" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1064" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1066" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1068" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1070" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1072" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1074" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1076" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1078" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1080" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1082" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1084" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1086" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1088" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1090" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1092" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1094" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1096" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1098" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1114" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1948,15 +3302,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
       <c r="A2" s="78" t="s">
@@ -2160,15 +3514,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
       <c r="A2" s="78" t="s">
@@ -2372,15 +3726,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" thickBot="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:5" ht="16" thickTop="1">
       <c r="A2" s="78" t="s">
@@ -2594,21 +3948,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" t="s">
@@ -3933,21 +5287,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="86" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
     </row>
     <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" t="s">
@@ -5287,21 +6641,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="16" thickBot="1">
       <c r="A2" s="44" t="s">
@@ -9296,30 +10650,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="8.5" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="84" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
     </row>
     <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="44" t="s">
@@ -9329,39 +10695,39 @@
         <v>2</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F2" s="47" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" thickTop="1">
       <c r="A3" s="34" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>8</v>
@@ -9393,10 +10759,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C4" s="55" t="s">
         <v>6</v>
@@ -9428,10 +10794,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C5" s="55" t="s">
         <v>7</v>
@@ -9463,10 +10829,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>6</v>
@@ -9498,10 +10864,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C7" s="55" t="s">
         <v>18</v>
@@ -9533,10 +10899,10 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>7</v>
@@ -9568,10 +10934,10 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C9" s="55" t="s">
         <v>7</v>
@@ -9603,10 +10969,10 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="17" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C10" s="55" t="s">
         <v>7</v>
@@ -9638,10 +11004,10 @@
     </row>
     <row r="11" spans="1:11" ht="16" thickBot="1">
       <c r="A11" s="33" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>7</v>
@@ -9673,63 +11039,63 @@
     </row>
     <row r="12" spans="1:11" ht="16" thickTop="1">
       <c r="A12" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C12" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="17">
-        <v>0</v>
-      </c>
-      <c r="F12" s="32">
-        <v>0</v>
-      </c>
-      <c r="G12" s="17">
-        <v>0</v>
-      </c>
-      <c r="H12" s="31">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17">
-        <v>0</v>
-      </c>
-      <c r="J12" s="17">
-        <v>0</v>
-      </c>
-      <c r="K12" s="31">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="32">
-        <v>0</v>
-      </c>
-      <c r="G13" s="17">
-        <v>0</v>
-      </c>
-      <c r="H13" s="31">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I13" s="60">
         <v>0</v>
@@ -9743,28 +11109,28 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="55">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="32">
-        <v>0</v>
-      </c>
-      <c r="G14" s="17">
-        <v>0</v>
-      </c>
-      <c r="H14" s="31">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I14" s="17">
         <v>0</v>
@@ -9778,28 +11144,28 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="31">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="31">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I15" s="17">
         <v>0</v>
@@ -9813,28 +11179,28 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C16" s="55" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="I16" s="17" t="s">
         <v>7</v>
@@ -9848,28 +11214,28 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C17" s="55" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="32">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>7</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>12</v>
+        <v>65</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>7</v>
@@ -9883,10 +11249,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C18" s="55" t="s">
         <v>7</v>
@@ -9901,7 +11267,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="H18" s="31" t="s">
         <v>7</v>
@@ -9918,10 +11284,10 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C19" s="55" t="s">
         <v>7</v>
@@ -9933,13 +11299,13 @@
         <v>7</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>12</v>
+        <v>64</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="I19" s="60" t="s">
         <v>7</v>
@@ -9953,10 +11319,10 @@
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="33" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C20" s="57" t="s">
         <v>7</v>
@@ -9988,10 +11354,10 @@
     </row>
     <row r="21" spans="1:11" ht="16" thickTop="1">
       <c r="A21" s="34" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C21" s="55" t="s">
         <v>7</v>
@@ -10023,10 +11389,10 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C22" s="55" t="s">
         <v>7</v>
@@ -10058,10 +11424,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C23" s="55" t="s">
         <v>7</v>
@@ -10093,10 +11459,10 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C24" s="55" t="s">
         <v>7</v>
@@ -10128,10 +11494,10 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B25" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C25" s="55" t="s">
         <v>7</v>
@@ -10163,10 +11529,10 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C26" s="55" t="s">
         <v>7</v>
@@ -10198,10 +11564,10 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C27" s="55" t="s">
         <v>7</v>
@@ -10233,10 +11599,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C28" s="55" t="s">
         <v>7</v>
@@ -10268,10 +11634,10 @@
     </row>
     <row r="29" spans="1:11" ht="16" thickBot="1">
       <c r="A29" s="33" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C29" s="57" t="s">
         <v>7</v>
@@ -10303,10 +11669,10 @@
     </row>
     <row r="30" spans="1:11" ht="16" thickTop="1">
       <c r="A30" s="34" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C30" s="51" t="s">
         <v>6</v>
@@ -10338,10 +11704,10 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C31" s="55" t="s">
         <v>18</v>
@@ -10373,10 +11739,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C32" s="55" t="s">
         <v>7</v>
@@ -10408,10 +11774,10 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C33" s="55" t="s">
         <v>18</v>
@@ -10443,10 +11809,10 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B34" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C34" s="55" t="s">
         <v>29</v>
@@ -10478,10 +11844,10 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B35" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C35" s="55" t="s">
         <v>7</v>
@@ -10513,10 +11879,10 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B36" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C36" s="55" t="s">
         <v>7</v>
@@ -10548,10 +11914,10 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B37" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C37" s="55" t="s">
         <v>7</v>
@@ -10583,10 +11949,10 @@
     </row>
     <row r="38" spans="1:11" ht="16" thickBot="1">
       <c r="A38" s="33" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B38" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C38" s="57" t="s">
         <v>7</v>
@@ -10618,63 +11984,63 @@
     </row>
     <row r="39" spans="1:11" ht="16" thickTop="1">
       <c r="A39" s="34" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="34">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>7</v>
       </c>
       <c r="F39" s="52" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="53">
-        <v>0</v>
-      </c>
-      <c r="I39" s="34">
-        <v>0</v>
-      </c>
-      <c r="J39" s="34">
-        <v>0</v>
-      </c>
-      <c r="K39" s="53">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="H39" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="53" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B40" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>7</v>
@@ -10688,28 +12054,28 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B41" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C41" s="55" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="F41" s="32" t="s">
         <v>7</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I41" s="60" t="s">
         <v>7</v>
@@ -10723,34 +12089,34 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B42" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="E42" s="31" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>7</v>
       </c>
       <c r="I42" s="60" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="J42" s="60" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="K42" s="31" t="s">
         <v>7</v>
@@ -10758,80 +12124,80 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B43" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C43" s="55" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>33</v>
+        <v>72</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I43" s="60" t="s">
-        <v>34</v>
+        <v>67</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>73</v>
       </c>
       <c r="J43" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="K43" s="31" t="s">
-        <v>35</v>
+        <v>72</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B44" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C44" s="55" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="F44" s="32" t="s">
         <v>7</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="H44" s="31" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="I44" s="60" t="s">
         <v>7</v>
       </c>
       <c r="J44" s="60" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="K44" s="31" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B45" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C45" s="55" t="s">
         <v>7</v>
@@ -10843,19 +12209,19 @@
         <v>7</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="H45" s="31" t="s">
         <v>7</v>
       </c>
       <c r="I45" s="60" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="J45" s="60" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="K45" s="31" t="s">
         <v>7</v>
@@ -10863,10 +12229,10 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="17" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B46" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C46" s="55" t="s">
         <v>7</v>
@@ -10878,30 +12244,30 @@
         <v>7</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="H46" s="31" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="I46" s="60" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="J46" s="60" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="16" thickBot="1">
       <c r="A47" s="33" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C47" s="57" t="s">
         <v>7</v>
@@ -10916,27 +12282,27 @@
         <v>7</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="H47" s="59" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="I47" s="33" t="s">
         <v>7</v>
       </c>
       <c r="J47" s="33" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="K47" s="59" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="16" thickTop="1">
       <c r="A48" s="34" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C48" s="51" t="s">
         <v>7</v>
@@ -10968,10 +12334,10 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B49" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C49" s="55" t="s">
         <v>7</v>
@@ -11003,10 +12369,10 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B50" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C50" s="55" t="s">
         <v>7</v>
@@ -11038,10 +12404,10 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B51" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C51" s="55" t="s">
         <v>7</v>
@@ -11073,10 +12439,10 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B52" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C52" s="55" t="s">
         <v>7</v>
@@ -11108,10 +12474,10 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B53" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C53" s="55" t="s">
         <v>7</v>
@@ -11143,10 +12509,10 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B54" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C54" s="55" t="s">
         <v>7</v>
@@ -11178,10 +12544,10 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="17" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B55" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C55" s="55" t="s">
         <v>7</v>
@@ -11213,10 +12579,10 @@
     </row>
     <row r="56" spans="1:11" ht="16" thickBot="1">
       <c r="A56" s="33" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B56" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C56" s="57" t="s">
         <v>7</v>
@@ -11248,10 +12614,10 @@
     </row>
     <row r="57" spans="1:11" ht="16" thickTop="1">
       <c r="A57" s="34" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C57" s="51">
         <v>0</v>
@@ -11283,10 +12649,10 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B58" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C58" s="55">
         <v>0</v>
@@ -11318,10 +12684,10 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B59" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C59" s="55">
         <v>0</v>
@@ -11353,10 +12719,10 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B60" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C60" s="55">
         <v>0</v>
@@ -11388,10 +12754,10 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B61" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C61" s="55">
         <v>0</v>
@@ -11423,10 +12789,10 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B62" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C62" s="55">
         <v>0</v>
@@ -11458,10 +12824,10 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B63" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C63" s="55">
         <v>0</v>
@@ -11493,10 +12859,10 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="17" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B64" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C64" s="55">
         <v>0</v>
@@ -11528,10 +12894,10 @@
     </row>
     <row r="65" spans="1:11" ht="16" thickBot="1">
       <c r="A65" s="33" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B65" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C65" s="57">
         <v>0</v>
@@ -11563,10 +12929,10 @@
     </row>
     <row r="66" spans="1:11" ht="16" thickTop="1">
       <c r="A66" s="34" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C66" s="51">
         <v>0</v>
@@ -11574,34 +12940,34 @@
       <c r="D66" s="34">
         <v>0</v>
       </c>
-      <c r="E66" s="53">
+      <c r="E66" s="34">
         <v>0</v>
       </c>
       <c r="F66" s="34" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="H66" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I66" s="34">
-        <v>0</v>
-      </c>
-      <c r="J66" s="34">
-        <v>0</v>
-      </c>
-      <c r="K66" s="53">
-        <v>0</v>
+      <c r="I66" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J66" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K66" s="53" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B67" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C67" s="55">
         <v>0</v>
@@ -11609,34 +12975,34 @@
       <c r="D67" s="17">
         <v>0</v>
       </c>
-      <c r="E67" s="31">
+      <c r="E67" s="17">
         <v>0</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="H67" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I67" s="60">
-        <v>0</v>
-      </c>
-      <c r="J67" s="60">
-        <v>0</v>
-      </c>
-      <c r="K67" s="31">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="I67" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K67" s="31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B68" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C68" s="55">
         <v>0</v>
@@ -11644,34 +13010,34 @@
       <c r="D68" s="17">
         <v>0</v>
       </c>
-      <c r="E68" s="31">
+      <c r="E68" s="17">
         <v>0</v>
       </c>
       <c r="F68" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H68" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I68" s="60">
-        <v>0</v>
-      </c>
-      <c r="J68" s="60">
-        <v>0</v>
-      </c>
-      <c r="K68" s="31">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="I68" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="K68" s="31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B69" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C69" s="55">
         <v>0</v>
@@ -11679,23 +13045,23 @@
       <c r="D69" s="17">
         <v>0</v>
       </c>
-      <c r="E69" s="31">
+      <c r="E69" s="17">
         <v>0</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H69" s="31" t="s">
         <v>7</v>
       </c>
       <c r="I69" s="60" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="J69" s="60" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="K69" s="31" t="s">
         <v>7</v>
@@ -11703,10 +13069,10 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B70" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C70" s="55">
         <v>0</v>
@@ -11714,34 +13080,34 @@
       <c r="D70" s="17">
         <v>0</v>
       </c>
-      <c r="E70" s="31">
+      <c r="E70" s="17">
         <v>0</v>
       </c>
       <c r="F70" s="60" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="G70" s="60" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="H70" s="31" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="I70" s="60" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="J70" s="60" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="K70" s="31" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C71" s="55">
         <v>0</v>
@@ -11749,34 +13115,34 @@
       <c r="D71" s="17">
         <v>0</v>
       </c>
-      <c r="E71" s="31">
+      <c r="E71" s="17">
         <v>0</v>
       </c>
       <c r="F71" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="H71" s="31" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="I71" s="32" t="s">
         <v>7</v>
       </c>
       <c r="J71" s="17" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="K71" s="31" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B72" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C72" s="55">
         <v>0</v>
@@ -11784,23 +13150,23 @@
       <c r="D72" s="17">
         <v>0</v>
       </c>
-      <c r="E72" s="31">
-        <v>0</v>
-      </c>
-      <c r="F72" s="17">
-        <v>0</v>
-      </c>
-      <c r="G72" s="17">
-        <v>0</v>
-      </c>
-      <c r="H72" s="31">
-        <v>0</v>
+      <c r="E72" s="17">
+        <v>0</v>
+      </c>
+      <c r="F72" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I72" s="32" t="s">
         <v>15</v>
       </c>
       <c r="J72" s="17" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K72" s="31" t="s">
         <v>7</v>
@@ -11808,10 +13174,10 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="17" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B73" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C73" s="55">
         <v>0</v>
@@ -11819,34 +13185,34 @@
       <c r="D73" s="17">
         <v>0</v>
       </c>
-      <c r="E73" s="31">
-        <v>0</v>
-      </c>
-      <c r="F73" s="17">
-        <v>0</v>
-      </c>
-      <c r="G73" s="17">
-        <v>0</v>
-      </c>
-      <c r="H73" s="31">
-        <v>0</v>
+      <c r="E73" s="17">
+        <v>0</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I73" s="32" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="K73" s="31" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="16" thickBot="1">
       <c r="A74" s="33" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B74" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C74" s="57">
         <v>0</v>
@@ -11854,17 +13220,17 @@
       <c r="D74" s="33">
         <v>0</v>
       </c>
-      <c r="E74" s="59">
-        <v>0</v>
-      </c>
-      <c r="F74" s="33">
-        <v>0</v>
-      </c>
-      <c r="G74" s="33">
-        <v>0</v>
-      </c>
-      <c r="H74" s="59">
-        <v>0</v>
+      <c r="E74" s="33">
+        <v>0</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" s="59" t="s">
+        <v>7</v>
       </c>
       <c r="I74" s="58" t="s">
         <v>7</v>
@@ -11873,15 +13239,15 @@
         <v>15</v>
       </c>
       <c r="K74" s="59" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="16" thickTop="1">
       <c r="A75" s="34" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C75" s="51">
         <v>0</v>
@@ -11913,10 +13279,10 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B76" s="54" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C76" s="55">
         <v>0</v>
@@ -11948,10 +13314,10 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B77" s="54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C77" s="55">
         <v>0</v>
@@ -11983,10 +13349,10 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B78" s="54" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C78" s="55">
         <v>0</v>
@@ -12018,10 +13384,10 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B79" s="54" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C79" s="55">
         <v>0</v>
@@ -12053,10 +13419,10 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B80" s="54" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C80" s="55">
         <v>0</v>
@@ -12088,10 +13454,10 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B81" s="54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C81" s="55">
         <v>0</v>
@@ -12123,10 +13489,10 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="17" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B82" s="54" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C82" s="55">
         <v>0</v>
@@ -12158,10 +13524,10 @@
     </row>
     <row r="83" spans="1:11" ht="16" thickBot="1">
       <c r="A83" s="33" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B83" s="56" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C83" s="57">
         <v>0</v>
@@ -12191,13 +13557,339 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="16" thickTop="1"/>
+    <row r="84" spans="1:11" ht="17" thickTop="1" thickBot="1"/>
+    <row r="85" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A85" s="82"/>
+      <c r="B85" s="83"/>
+    </row>
+    <row r="86" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A86" s="82"/>
+      <c r="B86" s="84"/>
+    </row>
+    <row r="87" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A87" s="82"/>
+      <c r="B87" s="84"/>
+    </row>
+    <row r="88" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A88" s="82"/>
+      <c r="B88" s="84"/>
+    </row>
+    <row r="89" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A89" s="82"/>
+      <c r="B89" s="84"/>
+    </row>
+    <row r="90" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A90" s="82"/>
+      <c r="B90" s="84"/>
+    </row>
+    <row r="91" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A91" s="82"/>
+      <c r="B91" s="84"/>
+    </row>
+    <row r="92" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A92" s="82"/>
+      <c r="B92" s="84"/>
+    </row>
+    <row r="93" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A93" s="82"/>
+      <c r="B93" s="85"/>
+    </row>
+    <row r="94" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A94" s="82"/>
+      <c r="B94" s="83"/>
+    </row>
+    <row r="95" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A95" s="82"/>
+      <c r="B95" s="84"/>
+    </row>
+    <row r="96" spans="1:11" ht="17" thickTop="1" thickBot="1">
+      <c r="A96" s="82"/>
+      <c r="B96" s="84"/>
+    </row>
+    <row r="97" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A97" s="82"/>
+      <c r="B97" s="84"/>
+    </row>
+    <row r="98" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A98" s="82"/>
+      <c r="B98" s="84"/>
+    </row>
+    <row r="99" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A99" s="82"/>
+      <c r="B99" s="84"/>
+    </row>
+    <row r="100" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A100" s="82"/>
+      <c r="B100" s="84"/>
+    </row>
+    <row r="101" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A101" s="82"/>
+      <c r="B101" s="84"/>
+    </row>
+    <row r="102" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A102" s="82"/>
+      <c r="B102" s="85"/>
+    </row>
+    <row r="103" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A103" s="82"/>
+      <c r="B103" s="83"/>
+    </row>
+    <row r="104" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A104" s="82"/>
+      <c r="B104" s="84"/>
+    </row>
+    <row r="105" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A105" s="82"/>
+      <c r="B105" s="84"/>
+    </row>
+    <row r="106" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A106" s="82"/>
+      <c r="B106" s="84"/>
+    </row>
+    <row r="107" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A107" s="82"/>
+      <c r="B107" s="84"/>
+    </row>
+    <row r="108" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A108" s="82"/>
+      <c r="B108" s="84"/>
+    </row>
+    <row r="109" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A109" s="82"/>
+      <c r="B109" s="84"/>
+    </row>
+    <row r="110" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A110" s="82"/>
+      <c r="B110" s="84"/>
+    </row>
+    <row r="111" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A111" s="82"/>
+      <c r="B111" s="85"/>
+    </row>
+    <row r="112" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A112" s="82"/>
+      <c r="B112" s="83"/>
+    </row>
+    <row r="113" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A113" s="82"/>
+      <c r="B113" s="84"/>
+    </row>
+    <row r="114" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A114" s="82"/>
+      <c r="B114" s="84"/>
+    </row>
+    <row r="115" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A115" s="82"/>
+      <c r="B115" s="84"/>
+    </row>
+    <row r="116" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A116" s="82"/>
+      <c r="B116" s="84"/>
+    </row>
+    <row r="117" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A117" s="82"/>
+      <c r="B117" s="84"/>
+    </row>
+    <row r="118" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A118" s="82"/>
+      <c r="B118" s="84"/>
+    </row>
+    <row r="119" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A119" s="82"/>
+      <c r="B119" s="84"/>
+    </row>
+    <row r="120" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A120" s="82"/>
+      <c r="B120" s="85"/>
+    </row>
+    <row r="121" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A121" s="82"/>
+      <c r="B121" s="83"/>
+    </row>
+    <row r="122" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A122" s="82"/>
+      <c r="B122" s="84"/>
+    </row>
+    <row r="123" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A123" s="82"/>
+      <c r="B123" s="84"/>
+    </row>
+    <row r="124" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A124" s="82"/>
+      <c r="B124" s="84"/>
+    </row>
+    <row r="125" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A125" s="82"/>
+      <c r="B125" s="84"/>
+    </row>
+    <row r="126" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A126" s="82"/>
+      <c r="B126" s="84"/>
+    </row>
+    <row r="127" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A127" s="82"/>
+      <c r="B127" s="84"/>
+    </row>
+    <row r="128" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A128" s="82"/>
+      <c r="B128" s="84"/>
+    </row>
+    <row r="129" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A129" s="82"/>
+      <c r="B129" s="85"/>
+    </row>
+    <row r="130" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A130" s="82"/>
+      <c r="B130" s="83"/>
+    </row>
+    <row r="131" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A131" s="82"/>
+      <c r="B131" s="84"/>
+    </row>
+    <row r="132" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A132" s="82"/>
+      <c r="B132" s="84"/>
+    </row>
+    <row r="133" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A133" s="82"/>
+      <c r="B133" s="84"/>
+    </row>
+    <row r="134" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A134" s="82"/>
+      <c r="B134" s="84"/>
+    </row>
+    <row r="135" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A135" s="82"/>
+      <c r="B135" s="84"/>
+    </row>
+    <row r="136" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A136" s="82"/>
+      <c r="B136" s="84"/>
+    </row>
+    <row r="137" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A137" s="82"/>
+      <c r="B137" s="84"/>
+    </row>
+    <row r="138" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A138" s="82"/>
+      <c r="B138" s="85"/>
+    </row>
+    <row r="139" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A139" s="82"/>
+      <c r="B139" s="83"/>
+    </row>
+    <row r="140" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A140" s="82"/>
+      <c r="B140" s="84"/>
+    </row>
+    <row r="141" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A141" s="82"/>
+      <c r="B141" s="84"/>
+    </row>
+    <row r="142" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A142" s="82"/>
+      <c r="B142" s="84"/>
+    </row>
+    <row r="143" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A143" s="82"/>
+      <c r="B143" s="84"/>
+    </row>
+    <row r="144" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A144" s="82"/>
+      <c r="B144" s="84"/>
+    </row>
+    <row r="145" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A145" s="82"/>
+      <c r="B145" s="84"/>
+    </row>
+    <row r="146" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A146" s="82"/>
+      <c r="B146" s="84"/>
+    </row>
+    <row r="147" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A147" s="82"/>
+      <c r="B147" s="85"/>
+    </row>
+    <row r="148" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A148" s="82"/>
+      <c r="B148" s="83"/>
+    </row>
+    <row r="149" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A149" s="82"/>
+      <c r="B149" s="84"/>
+    </row>
+    <row r="150" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A150" s="82"/>
+      <c r="B150" s="84"/>
+    </row>
+    <row r="151" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A151" s="82"/>
+      <c r="B151" s="84"/>
+    </row>
+    <row r="152" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A152" s="82"/>
+      <c r="B152" s="84"/>
+    </row>
+    <row r="153" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A153" s="82"/>
+      <c r="B153" s="84"/>
+    </row>
+    <row r="154" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A154" s="82"/>
+      <c r="B154" s="84"/>
+    </row>
+    <row r="155" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A155" s="82"/>
+      <c r="B155" s="84"/>
+    </row>
+    <row r="156" spans="1:2" s="36" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="A156" s="86"/>
+      <c r="B156" s="87"/>
+    </row>
+    <row r="157" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A157" s="82"/>
+      <c r="B157" s="83"/>
+    </row>
+    <row r="158" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A158" s="82"/>
+      <c r="B158" s="84"/>
+    </row>
+    <row r="159" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A159" s="82"/>
+      <c r="B159" s="84"/>
+    </row>
+    <row r="160" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A160" s="82"/>
+      <c r="B160" s="84"/>
+    </row>
+    <row r="161" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A161" s="82"/>
+      <c r="B161" s="84"/>
+    </row>
+    <row r="162" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A162" s="82"/>
+      <c r="B162" s="84"/>
+    </row>
+    <row r="163" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A163" s="82"/>
+      <c r="B163" s="84"/>
+    </row>
+    <row r="164" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A164" s="82"/>
+      <c r="B164" s="84"/>
+    </row>
+    <row r="165" spans="1:2" ht="17" thickTop="1" thickBot="1">
+      <c r="A165" s="82"/>
+      <c r="B165" s="85"/>
+    </row>
+    <row r="166" spans="1:2" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
yb changed model 7 to model 6prime also added Mathematica notebook
</commit_message>
<xml_diff>
--- a/writeup_and_notes/TransmissionRules.xlsx
+++ b/writeup_and_notes/TransmissionRules.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Model 4. Two-locus, coupling" sheetId="1" r:id="rId4"/>
     <sheet name="Model 5. Two-locus, repulsion" sheetId="3" r:id="rId5"/>
     <sheet name="Model 6. Two-locus, unlinked" sheetId="5" r:id="rId6"/>
-    <sheet name="Model 7. Two-locus unlinked fem" sheetId="10" r:id="rId7"/>
+    <sheet name="Model 6' Two-locus unlinked fem" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -10653,8 +10653,8 @@
   <dimension ref="A1:K166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>